<commit_message>
updated formula to more robust version
</commit_message>
<xml_diff>
--- a/STANDARD/CHEM-STND-003_Worksheet.xlsx
+++ b/STANDARD/CHEM-STND-003_Worksheet.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classifications (Reference Only" sheetId="1" state="visible" r:id="rId2"/>
@@ -346,6 +346,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -367,12 +368,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -575,10 +578,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -615,7 +614,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -639,7 +638,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -649,6 +648,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -775,10 +778,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="C62:J62 C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="74.61"/>
   </cols>
@@ -1020,11 +1023,11 @@
   </sheetPr>
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62:J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
@@ -2401,87 +2404,87 @@
         <v>42</v>
       </c>
       <c r="H53" s="19"/>
-      <c r="I53" s="20" t="s">
+      <c r="I53" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J53" s="20"/>
+      <c r="J53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="19" t="s">
         <v>90</v>
       </c>
       <c r="B54" s="19"/>
-      <c r="C54" s="21" t="n">
+      <c r="C54" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21" t="n">
+      <c r="D54" s="20"/>
+      <c r="E54" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21" t="n">
+      <c r="F54" s="20"/>
+      <c r="G54" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21" t="n">
+      <c r="H54" s="20"/>
+      <c r="I54" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="J54" s="21"/>
+      <c r="J54" s="20"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="18"/>
-      <c r="C55" s="22"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="18"/>
-      <c r="E55" s="22"/>
+      <c r="E55" s="21"/>
       <c r="F55" s="18"/>
-      <c r="G55" s="22"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="18"/>
-      <c r="I55" s="23"/>
+      <c r="I55" s="22"/>
       <c r="J55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="18"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="18"/>
-      <c r="E56" s="22"/>
+      <c r="E56" s="21"/>
       <c r="F56" s="18"/>
-      <c r="G56" s="22"/>
+      <c r="G56" s="21"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="23"/>
+      <c r="I56" s="22"/>
       <c r="J56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="14"/>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="14"/>
       <c r="C59" s="19" t="s">
         <v>38</v>
@@ -2495,42 +2498,42 @@
         <v>42</v>
       </c>
       <c r="H59" s="19"/>
-      <c r="I59" s="27" t="s">
+      <c r="I59" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J59" s="27"/>
+      <c r="J59" s="26"/>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="29" t="n">
+      <c r="B60" s="27"/>
+      <c r="C60" s="28" t="n">
         <f aca="false">100*C54/SUM($C$54:$I$54)</f>
         <v>25</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29" t="n">
+      <c r="D60" s="28"/>
+      <c r="E60" s="28" t="n">
         <f aca="false">100*E54/SUM($C$54:$I$54)</f>
         <v>25</v>
       </c>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29" t="n">
+      <c r="F60" s="28"/>
+      <c r="G60" s="28" t="n">
         <f aca="false">100*G54/SUM($C$54:$I$54)</f>
         <v>25</v>
       </c>
-      <c r="H60" s="29"/>
-      <c r="I60" s="30" t="n">
+      <c r="H60" s="28"/>
+      <c r="I60" s="29" t="n">
         <f aca="false">100*I54/SUM($C$54:$I$54)</f>
         <v>25</v>
       </c>
-      <c r="J60" s="30"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -2538,225 +2541,225 @@
       <c r="G61" s="18"/>
       <c r="H61" s="14"/>
       <c r="I61" s="18"/>
-      <c r="J61" s="32"/>
+      <c r="J61" s="31"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="33"/>
-      <c r="B62" s="34" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="19" t="n">
-        <f aca="false">COUNTIF(C4:C50,"&lt;&gt;Impossible")-COUNTIFS(C4:C50,"&lt;&gt;[:alpha:]*")</f>
+      <c r="C62" s="34" t="n">
+        <f aca="false">COUNTIF(C4:C51,"&lt;&gt;Impossible")-COUNTBLANK(C4:C51)</f>
         <v>1</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19" t="n">
-        <f aca="false">COUNTIF(E4:E50,"&lt;&gt;Impossible")-COUNTIFS(E4:E50,"&lt;&gt;[:alpha:]*")</f>
-        <v>0</v>
-      </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19" t="n">
-        <f aca="false">COUNTIF(G4:G50,"&lt;&gt;Impossible")-COUNTIFS(G4:G50,"&lt;&gt;[:alpha:]*")</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="19"/>
-      <c r="I62" s="27" t="n">
-        <f aca="false">COUNTIF(I4:I50,"&lt;&gt;Impossible")-COUNTIFS(I4:I50,"&lt;&gt;[:alpha:]*")</f>
-        <v>0</v>
-      </c>
-      <c r="J62" s="27"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34" t="n">
+        <f aca="false">COUNTIF(E4:E51,"&lt;&gt;Impossible")-COUNTBLANK(E4:E51)</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34" t="n">
+        <f aca="false">COUNTIF(G4:G51,"&lt;&gt;Impossible")-COUNTBLANK(G4:G51)</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34" t="n">
+        <f aca="false">COUNTIF(I4:I51,"&lt;&gt;Impossible")-COUNTBLANK(I4:I51)</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="34"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="33"/>
-      <c r="B63" s="34" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="35" t="n">
+      <c r="C63" s="28" t="n">
         <f aca="false">100*C62/SUM($C$62:$I$62)</f>
         <v>100</v>
       </c>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35" t="n">
+      <c r="D63" s="28"/>
+      <c r="E63" s="28" t="n">
         <f aca="false">100*E62/SUM($C$62:$I$62)</f>
         <v>0</v>
       </c>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35" t="n">
+      <c r="F63" s="28"/>
+      <c r="G63" s="28" t="n">
         <f aca="false">100*G62/SUM($C$62:$I$62)</f>
         <v>0</v>
       </c>
-      <c r="H63" s="35"/>
-      <c r="I63" s="30" t="n">
+      <c r="H63" s="28"/>
+      <c r="I63" s="29" t="n">
         <f aca="false">100*I62/SUM($C$62:$I$62)</f>
         <v>0</v>
       </c>
-      <c r="J63" s="30"/>
+      <c r="J63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="33"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="37"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="36"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="29" t="n">
+      <c r="B65" s="30"/>
+      <c r="C65" s="28" t="n">
         <f aca="false">(C60+C63)</f>
         <v>125</v>
       </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29" t="n">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28" t="n">
         <f aca="false">(E60+E63)</f>
         <v>25</v>
       </c>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29" t="n">
+      <c r="F65" s="28"/>
+      <c r="G65" s="28" t="n">
         <f aca="false">(G60+G63)</f>
         <v>25</v>
       </c>
-      <c r="H65" s="29"/>
-      <c r="I65" s="30" t="n">
+      <c r="H65" s="28"/>
+      <c r="I65" s="29" t="n">
         <f aca="false">(I60+I63)</f>
         <v>25</v>
       </c>
-      <c r="J65" s="30"/>
+      <c r="J65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="29" t="n">
+      <c r="B66" s="30"/>
+      <c r="C66" s="28" t="n">
         <f aca="false">ABS(C63-C60)</f>
         <v>75</v>
       </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29" t="n">
+      <c r="D66" s="28"/>
+      <c r="E66" s="28" t="n">
         <f aca="false">ABS(E63-E60)</f>
         <v>25</v>
       </c>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29" t="n">
+      <c r="F66" s="28"/>
+      <c r="G66" s="28" t="n">
         <f aca="false">ABS(G63-G60)</f>
         <v>25</v>
       </c>
-      <c r="H66" s="29"/>
-      <c r="I66" s="30" t="n">
+      <c r="H66" s="28"/>
+      <c r="I66" s="29" t="n">
         <f aca="false">ABS(I63-I60)</f>
         <v>25</v>
       </c>
-      <c r="J66" s="30"/>
+      <c r="J66" s="29"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="29" t="n">
+      <c r="B67" s="30"/>
+      <c r="C67" s="28" t="n">
         <f aca="false">1-C66/C65</f>
         <v>0.4</v>
       </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29" t="n">
+      <c r="D67" s="28"/>
+      <c r="E67" s="28" t="n">
         <f aca="false">1-E66/E65</f>
         <v>0</v>
       </c>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29" t="n">
+      <c r="F67" s="28"/>
+      <c r="G67" s="28" t="n">
         <f aca="false">1-G66/G65</f>
         <v>0</v>
       </c>
-      <c r="H67" s="29"/>
-      <c r="I67" s="30" t="n">
+      <c r="H67" s="28"/>
+      <c r="I67" s="29" t="n">
         <f aca="false">1-I66/I65</f>
         <v>0</v>
       </c>
-      <c r="J67" s="30"/>
+      <c r="J67" s="29"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="18"/>
-      <c r="C68" s="29"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="38"/>
-      <c r="E68" s="29"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="38"/>
-      <c r="G68" s="29"/>
+      <c r="G68" s="37"/>
       <c r="H68" s="38"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="36"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="39" t="s">
         <v>99</v>
       </c>
       <c r="B69" s="39"/>
-      <c r="C69" s="29" t="n">
+      <c r="C69" s="28" t="n">
         <f aca="false">SUM(D4:D50)</f>
         <v>1</v>
       </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29" t="n">
+      <c r="D69" s="28"/>
+      <c r="E69" s="28" t="n">
         <f aca="false">SUM(F4:F50)</f>
         <v>0</v>
       </c>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29" t="n">
+      <c r="F69" s="28"/>
+      <c r="G69" s="28" t="n">
         <f aca="false">SUM(H4:H50)</f>
         <v>0</v>
       </c>
-      <c r="H69" s="29"/>
-      <c r="I69" s="30" t="n">
+      <c r="H69" s="28"/>
+      <c r="I69" s="29" t="n">
         <f aca="false">SUM(J4:J50)</f>
         <v>0</v>
       </c>
-      <c r="J69" s="30"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="39" t="s">
         <v>100</v>
       </c>
       <c r="B70" s="39"/>
-      <c r="C70" s="29" t="n">
+      <c r="C70" s="28" t="n">
         <f aca="false">C69*C67</f>
         <v>0.4</v>
       </c>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29" t="n">
+      <c r="D70" s="28"/>
+      <c r="E70" s="28" t="n">
         <f aca="false">E69*E67</f>
         <v>0</v>
       </c>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29" t="n">
+      <c r="F70" s="28"/>
+      <c r="G70" s="28" t="n">
         <f aca="false">G69*G67</f>
         <v>0</v>
       </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="30" t="n">
+      <c r="H70" s="28"/>
+      <c r="I70" s="29" t="n">
         <f aca="false">I69*I67</f>
         <v>0</v>
       </c>
-      <c r="J70" s="30"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="33"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="18"/>
-      <c r="C71" s="22"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="18"/>
-      <c r="E71" s="22"/>
+      <c r="E71" s="21"/>
       <c r="F71" s="18"/>
-      <c r="G71" s="22"/>
+      <c r="G71" s="21"/>
       <c r="H71" s="18"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="32"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="31"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="40" t="s">
@@ -2840,11 +2843,11 @@
     <mergeCell ref="C72:J72"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4 G4 I4 C7:C11 E7:E11 G7:G11 I7:I11 C14:C16 E14:E16 G14:G16 I14:I16 C19:C22 E19:E22 G19:G22 I19:I22 C25:C29 E25:E29 G25:G29 I25:I29 C32 E32 G32 I32 C35:C39 E35:E39 G35:G39 I35:I39 C42:C45 E42:E45 G42:G45 I42:I45 C48:C51 E48:E51 G48:G51 I48:I51" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4" type="list">
       <formula1>'Classifications (Reference Only'!$B$2:$B$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4 G4 I4 C7:C11 E7:E11 G7:G11 I7:I11 C14:C16 E14:E16 G14:G16 I14:I16 C19:C22 E19:E22 G19:G22 I19:I22 C25:C29 E25:E29 G25:G29 I25:I29 C32 E32 G32 I32 C35:C39 E35:E39 G35:G39 I35:I39 C42:C45 E42:E45 G42:G45 I42:I45 C48:C51 E48:E51 G48:G51 I48:I51" type="list">
       <formula1>'Classifications (Reference Only'!$B$2:$B$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2866,13 +2869,13 @@
   </sheetPr>
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62:J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4250,87 +4253,87 @@
         <v>42</v>
       </c>
       <c r="H53" s="19"/>
-      <c r="I53" s="20" t="s">
+      <c r="I53" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J53" s="20"/>
+      <c r="J53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="19" t="s">
         <v>90</v>
       </c>
       <c r="B54" s="19"/>
-      <c r="C54" s="21" t="n">
+      <c r="C54" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21" t="n">
+      <c r="D54" s="20"/>
+      <c r="E54" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21" t="n">
+      <c r="F54" s="20"/>
+      <c r="G54" s="20" t="n">
         <v>30</v>
       </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21" t="n">
+      <c r="H54" s="20"/>
+      <c r="I54" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="J54" s="21"/>
+      <c r="J54" s="20"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="18"/>
-      <c r="C55" s="22"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="18"/>
-      <c r="E55" s="22"/>
+      <c r="E55" s="21"/>
       <c r="F55" s="18"/>
-      <c r="G55" s="22"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="18"/>
-      <c r="I55" s="23"/>
+      <c r="I55" s="22"/>
       <c r="J55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="18"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="18"/>
-      <c r="E56" s="22"/>
+      <c r="E56" s="21"/>
       <c r="F56" s="18"/>
-      <c r="G56" s="22"/>
+      <c r="G56" s="21"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="23"/>
+      <c r="I56" s="22"/>
       <c r="J56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="14"/>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="14"/>
       <c r="C59" s="19" t="s">
         <v>38</v>
@@ -4344,42 +4347,42 @@
         <v>42</v>
       </c>
       <c r="H59" s="19"/>
-      <c r="I59" s="27" t="s">
+      <c r="I59" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J59" s="27"/>
+      <c r="J59" s="26"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="29" t="n">
+      <c r="B60" s="27"/>
+      <c r="C60" s="28" t="n">
         <f aca="false">100*C54/SUM($C$54:$I$54)</f>
         <v>5</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29" t="n">
+      <c r="D60" s="28"/>
+      <c r="E60" s="28" t="n">
         <f aca="false">100*E54/SUM($C$54:$I$54)</f>
         <v>25</v>
       </c>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29" t="n">
+      <c r="F60" s="28"/>
+      <c r="G60" s="28" t="n">
         <f aca="false">100*G54/SUM($C$54:$I$54)</f>
         <v>30</v>
       </c>
-      <c r="H60" s="29"/>
-      <c r="I60" s="30" t="n">
+      <c r="H60" s="28"/>
+      <c r="I60" s="29" t="n">
         <f aca="false">100*I54/SUM($C$54:$I$54)</f>
         <v>40</v>
       </c>
-      <c r="J60" s="30"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -4387,11 +4390,11 @@
       <c r="G61" s="18"/>
       <c r="H61" s="14"/>
       <c r="I61" s="18"/>
-      <c r="J61" s="32"/>
+      <c r="J61" s="31"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="33"/>
-      <c r="B62" s="34" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="33" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="19" t="n">
@@ -4409,203 +4412,203 @@
         <v>22</v>
       </c>
       <c r="H62" s="19"/>
-      <c r="I62" s="27" t="n">
+      <c r="I62" s="26" t="n">
         <f aca="false">COUNTIF(I4:I50,"&lt;&gt;Impossible")-COUNTIFS(I4:I50,"&lt;&gt;[:alpha:]*")</f>
         <v>25</v>
       </c>
-      <c r="J62" s="27"/>
+      <c r="J62" s="26"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="33"/>
-      <c r="B63" s="34" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="35" t="n">
+      <c r="C63" s="28" t="n">
         <f aca="false">100*C62/SUM($C$62:$I$62)</f>
         <v>5</v>
       </c>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35" t="n">
+      <c r="D63" s="28"/>
+      <c r="E63" s="28" t="n">
         <f aca="false">100*E62/SUM($C$62:$I$62)</f>
         <v>16.6666666666667</v>
       </c>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35" t="n">
+      <c r="F63" s="28"/>
+      <c r="G63" s="28" t="n">
         <f aca="false">100*G62/SUM($C$62:$I$62)</f>
         <v>36.6666666666667</v>
       </c>
-      <c r="H63" s="35"/>
-      <c r="I63" s="30" t="n">
+      <c r="H63" s="28"/>
+      <c r="I63" s="29" t="n">
         <f aca="false">100*I62/SUM($C$62:$I$62)</f>
         <v>41.6666666666667</v>
       </c>
-      <c r="J63" s="30"/>
+      <c r="J63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="33"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="37"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="36"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="29" t="n">
+      <c r="B65" s="30"/>
+      <c r="C65" s="28" t="n">
         <f aca="false">(C60+C63)</f>
         <v>10</v>
       </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29" t="n">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28" t="n">
         <f aca="false">(E60+E63)</f>
         <v>41.6666666666667</v>
       </c>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29" t="n">
+      <c r="F65" s="28"/>
+      <c r="G65" s="28" t="n">
         <f aca="false">(G60+G63)</f>
         <v>66.6666666666667</v>
       </c>
-      <c r="H65" s="29"/>
-      <c r="I65" s="30" t="n">
+      <c r="H65" s="28"/>
+      <c r="I65" s="29" t="n">
         <f aca="false">(I60+I63)</f>
         <v>81.6666666666667</v>
       </c>
-      <c r="J65" s="30"/>
+      <c r="J65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="29" t="n">
+      <c r="B66" s="30"/>
+      <c r="C66" s="28" t="n">
         <f aca="false">ABS(C63-C60)</f>
         <v>0</v>
       </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29" t="n">
+      <c r="D66" s="28"/>
+      <c r="E66" s="28" t="n">
         <f aca="false">ABS(E63-E60)</f>
         <v>8.33333333333333</v>
       </c>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29" t="n">
+      <c r="F66" s="28"/>
+      <c r="G66" s="28" t="n">
         <f aca="false">ABS(G63-G60)</f>
         <v>6.66666666666666</v>
       </c>
-      <c r="H66" s="29"/>
-      <c r="I66" s="30" t="n">
+      <c r="H66" s="28"/>
+      <c r="I66" s="29" t="n">
         <f aca="false">ABS(I63-I60)</f>
         <v>1.66666666666666</v>
       </c>
-      <c r="J66" s="30"/>
+      <c r="J66" s="29"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="29" t="n">
+      <c r="B67" s="30"/>
+      <c r="C67" s="28" t="n">
         <f aca="false">1-C66/C65</f>
         <v>1</v>
       </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29" t="n">
+      <c r="D67" s="28"/>
+      <c r="E67" s="28" t="n">
         <f aca="false">1-E66/E65</f>
         <v>0.8</v>
       </c>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29" t="n">
+      <c r="F67" s="28"/>
+      <c r="G67" s="28" t="n">
         <f aca="false">1-G66/G65</f>
         <v>0.9</v>
       </c>
-      <c r="H67" s="29"/>
-      <c r="I67" s="30" t="n">
+      <c r="H67" s="28"/>
+      <c r="I67" s="29" t="n">
         <f aca="false">1-I66/I65</f>
         <v>0.979591836734694</v>
       </c>
-      <c r="J67" s="30"/>
+      <c r="J67" s="29"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="18"/>
-      <c r="C68" s="29"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="38"/>
-      <c r="E68" s="29"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="38"/>
-      <c r="G68" s="29"/>
+      <c r="G68" s="37"/>
       <c r="H68" s="38"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="36"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="39" t="s">
         <v>99</v>
       </c>
       <c r="B69" s="39"/>
-      <c r="C69" s="29" t="n">
+      <c r="C69" s="28" t="n">
         <f aca="false">SUM(D4:D50)</f>
         <v>9</v>
       </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29" t="n">
+      <c r="D69" s="28"/>
+      <c r="E69" s="28" t="n">
         <f aca="false">SUM(F4:F50)</f>
         <v>27</v>
       </c>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29" t="n">
+      <c r="F69" s="28"/>
+      <c r="G69" s="28" t="n">
         <f aca="false">SUM(H4:H50)</f>
         <v>54</v>
       </c>
-      <c r="H69" s="29"/>
-      <c r="I69" s="30" t="n">
+      <c r="H69" s="28"/>
+      <c r="I69" s="29" t="n">
         <f aca="false">SUM(J4:J50)</f>
         <v>65</v>
       </c>
-      <c r="J69" s="30"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="39" t="s">
         <v>100</v>
       </c>
       <c r="B70" s="39"/>
-      <c r="C70" s="29" t="n">
+      <c r="C70" s="28" t="n">
         <f aca="false">C69*C67</f>
         <v>9</v>
       </c>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29" t="n">
+      <c r="D70" s="28"/>
+      <c r="E70" s="28" t="n">
         <f aca="false">E69*E67</f>
         <v>21.6</v>
       </c>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29" t="n">
+      <c r="F70" s="28"/>
+      <c r="G70" s="28" t="n">
         <f aca="false">G69*G67</f>
         <v>48.6</v>
       </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="30" t="n">
+      <c r="H70" s="28"/>
+      <c r="I70" s="29" t="n">
         <f aca="false">I69*I67</f>
         <v>63.6734693877551</v>
       </c>
-      <c r="J70" s="30"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="33"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="18"/>
-      <c r="C71" s="22"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="18"/>
-      <c r="E71" s="22"/>
+      <c r="E71" s="21"/>
       <c r="F71" s="18"/>
-      <c r="G71" s="22"/>
+      <c r="G71" s="21"/>
       <c r="H71" s="18"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="32"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="31"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="40" t="s">
@@ -4716,12 +4719,12 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="C62:J62 E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6097,87 +6100,87 @@
         <v>42</v>
       </c>
       <c r="H53" s="19"/>
-      <c r="I53" s="20" t="s">
+      <c r="I53" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J53" s="20"/>
+      <c r="J53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="19" t="s">
         <v>90</v>
       </c>
       <c r="B54" s="19"/>
-      <c r="C54" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21" t="n">
+      <c r="C54" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21" t="n">
+      <c r="F54" s="20"/>
+      <c r="G54" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21" t="n">
+      <c r="H54" s="20"/>
+      <c r="I54" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="J54" s="21"/>
+      <c r="J54" s="20"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="18"/>
-      <c r="C55" s="22"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="18"/>
-      <c r="E55" s="22"/>
+      <c r="E55" s="21"/>
       <c r="F55" s="18"/>
-      <c r="G55" s="22"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="18"/>
-      <c r="I55" s="23"/>
+      <c r="I55" s="22"/>
       <c r="J55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="18"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="18"/>
-      <c r="E56" s="22"/>
+      <c r="E56" s="21"/>
       <c r="F56" s="18"/>
-      <c r="G56" s="22"/>
+      <c r="G56" s="21"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="23"/>
+      <c r="I56" s="22"/>
       <c r="J56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="14"/>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="14"/>
       <c r="C59" s="19" t="s">
         <v>38</v>
@@ -6191,42 +6194,42 @@
         <v>42</v>
       </c>
       <c r="H59" s="19"/>
-      <c r="I59" s="27" t="s">
+      <c r="I59" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J59" s="27"/>
+      <c r="J59" s="26"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="29" t="n">
+      <c r="B60" s="27"/>
+      <c r="C60" s="28" t="n">
         <f aca="false">100*C54/SUM($C$54:$I$54)</f>
         <v>0</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29" t="n">
+      <c r="D60" s="28"/>
+      <c r="E60" s="28" t="n">
         <f aca="false">100*E54/SUM($C$54:$I$54)</f>
         <v>5</v>
       </c>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29" t="n">
+      <c r="F60" s="28"/>
+      <c r="G60" s="28" t="n">
         <f aca="false">100*G54/SUM($C$54:$I$54)</f>
         <v>45</v>
       </c>
-      <c r="H60" s="29"/>
-      <c r="I60" s="30" t="n">
+      <c r="H60" s="28"/>
+      <c r="I60" s="29" t="n">
         <f aca="false">100*I54/SUM($C$54:$I$54)</f>
         <v>50</v>
       </c>
-      <c r="J60" s="30"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -6234,11 +6237,11 @@
       <c r="G61" s="18"/>
       <c r="H61" s="14"/>
       <c r="I61" s="18"/>
-      <c r="J61" s="32"/>
+      <c r="J61" s="31"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="33"/>
-      <c r="B62" s="34" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="33" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="19" t="n">
@@ -6256,203 +6259,203 @@
         <v>22</v>
       </c>
       <c r="H62" s="19"/>
-      <c r="I62" s="27" t="n">
+      <c r="I62" s="26" t="n">
         <f aca="false">COUNTIF(I4:I50,"&lt;&gt;Impossible")-COUNTIFS(I4:I50,"&lt;&gt;[:alpha:]*")</f>
         <v>25</v>
       </c>
-      <c r="J62" s="27"/>
+      <c r="J62" s="26"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="33"/>
-      <c r="B63" s="34" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="35" t="n">
+      <c r="C63" s="28" t="n">
         <f aca="false">100*C62/SUM($C$62:$I$62)</f>
         <v>5</v>
       </c>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35" t="n">
+      <c r="D63" s="28"/>
+      <c r="E63" s="28" t="n">
         <f aca="false">100*E62/SUM($C$62:$I$62)</f>
         <v>16.6666666666667</v>
       </c>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35" t="n">
+      <c r="F63" s="28"/>
+      <c r="G63" s="28" t="n">
         <f aca="false">100*G62/SUM($C$62:$I$62)</f>
         <v>36.6666666666667</v>
       </c>
-      <c r="H63" s="35"/>
-      <c r="I63" s="30" t="n">
+      <c r="H63" s="28"/>
+      <c r="I63" s="29" t="n">
         <f aca="false">100*I62/SUM($C$62:$I$62)</f>
         <v>41.6666666666667</v>
       </c>
-      <c r="J63" s="30"/>
+      <c r="J63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="33"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="37"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="36"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="29" t="n">
+      <c r="B65" s="30"/>
+      <c r="C65" s="28" t="n">
         <f aca="false">(C60+C63)</f>
         <v>5</v>
       </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29" t="n">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28" t="n">
         <f aca="false">(E60+E63)</f>
         <v>21.6666666666667</v>
       </c>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29" t="n">
+      <c r="F65" s="28"/>
+      <c r="G65" s="28" t="n">
         <f aca="false">(G60+G63)</f>
         <v>81.6666666666667</v>
       </c>
-      <c r="H65" s="29"/>
-      <c r="I65" s="30" t="n">
+      <c r="H65" s="28"/>
+      <c r="I65" s="29" t="n">
         <f aca="false">(I60+I63)</f>
         <v>91.6666666666667</v>
       </c>
-      <c r="J65" s="30"/>
+      <c r="J65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="29" t="n">
+      <c r="B66" s="30"/>
+      <c r="C66" s="28" t="n">
         <f aca="false">ABS(C63-C60)</f>
         <v>5</v>
       </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29" t="n">
+      <c r="D66" s="28"/>
+      <c r="E66" s="28" t="n">
         <f aca="false">ABS(E63-E60)</f>
         <v>11.6666666666667</v>
       </c>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29" t="n">
+      <c r="F66" s="28"/>
+      <c r="G66" s="28" t="n">
         <f aca="false">ABS(G63-G60)</f>
         <v>8.33333333333334</v>
       </c>
-      <c r="H66" s="29"/>
-      <c r="I66" s="30" t="n">
+      <c r="H66" s="28"/>
+      <c r="I66" s="29" t="n">
         <f aca="false">ABS(I63-I60)</f>
         <v>8.33333333333334</v>
       </c>
-      <c r="J66" s="30"/>
+      <c r="J66" s="29"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="29" t="n">
+      <c r="B67" s="30"/>
+      <c r="C67" s="28" t="n">
         <f aca="false">1-C66/C65</f>
         <v>0</v>
       </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29" t="n">
+      <c r="D67" s="28"/>
+      <c r="E67" s="28" t="n">
         <f aca="false">1-E66/E65</f>
         <v>0.461538461538462</v>
       </c>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29" t="n">
+      <c r="F67" s="28"/>
+      <c r="G67" s="28" t="n">
         <f aca="false">1-G66/G65</f>
         <v>0.897959183673469</v>
       </c>
-      <c r="H67" s="29"/>
-      <c r="I67" s="30" t="n">
+      <c r="H67" s="28"/>
+      <c r="I67" s="29" t="n">
         <f aca="false">1-I66/I65</f>
         <v>0.909090909090909</v>
       </c>
-      <c r="J67" s="30"/>
+      <c r="J67" s="29"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="18"/>
-      <c r="C68" s="29"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="38"/>
-      <c r="E68" s="29"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="38"/>
-      <c r="G68" s="29"/>
+      <c r="G68" s="37"/>
       <c r="H68" s="38"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="36"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="39" t="s">
         <v>99</v>
       </c>
       <c r="B69" s="39"/>
-      <c r="C69" s="29" t="n">
+      <c r="C69" s="28" t="n">
         <f aca="false">SUM(D4:D50)</f>
         <v>3</v>
       </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29" t="n">
+      <c r="D69" s="28"/>
+      <c r="E69" s="28" t="n">
         <f aca="false">SUM(F4:F50)</f>
         <v>15</v>
       </c>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29" t="n">
+      <c r="F69" s="28"/>
+      <c r="G69" s="28" t="n">
         <f aca="false">SUM(H4:H50)</f>
         <v>64</v>
       </c>
-      <c r="H69" s="29"/>
-      <c r="I69" s="30" t="n">
+      <c r="H69" s="28"/>
+      <c r="I69" s="29" t="n">
         <f aca="false">SUM(J4:J50)</f>
         <v>71</v>
       </c>
-      <c r="J69" s="30"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="39" t="s">
         <v>100</v>
       </c>
       <c r="B70" s="39"/>
-      <c r="C70" s="29" t="n">
+      <c r="C70" s="28" t="n">
         <f aca="false">C69*C67</f>
         <v>0</v>
       </c>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29" t="n">
+      <c r="D70" s="28"/>
+      <c r="E70" s="28" t="n">
         <f aca="false">E69*E67</f>
         <v>6.92307692307692</v>
       </c>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29" t="n">
+      <c r="F70" s="28"/>
+      <c r="G70" s="28" t="n">
         <f aca="false">G69*G67</f>
         <v>57.469387755102</v>
       </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="30" t="n">
+      <c r="H70" s="28"/>
+      <c r="I70" s="29" t="n">
         <f aca="false">I69*I67</f>
         <v>64.5454545454546</v>
       </c>
-      <c r="J70" s="30"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="33"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="18"/>
-      <c r="C71" s="22"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="18"/>
-      <c r="E71" s="22"/>
+      <c r="E71" s="21"/>
       <c r="F71" s="18"/>
-      <c r="G71" s="22"/>
+      <c r="G71" s="21"/>
       <c r="H71" s="18"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="32"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="31"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="40" t="s">
@@ -6563,12 +6566,12 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="1" sqref="C62:J62 E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7946,87 +7949,87 @@
         <v>42</v>
       </c>
       <c r="H53" s="19"/>
-      <c r="I53" s="20" t="s">
+      <c r="I53" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J53" s="20"/>
+      <c r="J53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="19" t="s">
         <v>90</v>
       </c>
       <c r="B54" s="19"/>
-      <c r="C54" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21" t="n">
+      <c r="C54" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21" t="n">
+      <c r="H54" s="20"/>
+      <c r="I54" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="J54" s="21"/>
+      <c r="J54" s="20"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="18"/>
-      <c r="C55" s="22"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="18"/>
-      <c r="E55" s="22"/>
+      <c r="E55" s="21"/>
       <c r="F55" s="18"/>
-      <c r="G55" s="22"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="18"/>
-      <c r="I55" s="23"/>
+      <c r="I55" s="22"/>
       <c r="J55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="18"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="18"/>
-      <c r="E56" s="22"/>
+      <c r="E56" s="21"/>
       <c r="F56" s="18"/>
-      <c r="G56" s="22"/>
+      <c r="G56" s="21"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="23"/>
+      <c r="I56" s="22"/>
       <c r="J56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="14"/>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="14"/>
       <c r="C59" s="19" t="s">
         <v>38</v>
@@ -8040,42 +8043,42 @@
         <v>42</v>
       </c>
       <c r="H59" s="19"/>
-      <c r="I59" s="27" t="s">
+      <c r="I59" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J59" s="27"/>
+      <c r="J59" s="26"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="29" t="n">
+      <c r="B60" s="27"/>
+      <c r="C60" s="28" t="n">
         <f aca="false">100*C54/SUM($C$54:$I$54)</f>
         <v>0</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29" t="n">
+      <c r="D60" s="28"/>
+      <c r="E60" s="28" t="n">
         <f aca="false">100*E54/SUM($C$54:$I$54)</f>
         <v>0</v>
       </c>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29" t="n">
+      <c r="F60" s="28"/>
+      <c r="G60" s="28" t="n">
         <f aca="false">100*G54/SUM($C$54:$I$54)</f>
         <v>50</v>
       </c>
-      <c r="H60" s="29"/>
-      <c r="I60" s="30" t="n">
+      <c r="H60" s="28"/>
+      <c r="I60" s="29" t="n">
         <f aca="false">100*I54/SUM($C$54:$I$54)</f>
         <v>50</v>
       </c>
-      <c r="J60" s="30"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -8083,11 +8086,11 @@
       <c r="G61" s="18"/>
       <c r="H61" s="14"/>
       <c r="I61" s="18"/>
-      <c r="J61" s="32"/>
+      <c r="J61" s="31"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="33"/>
-      <c r="B62" s="34" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="33" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="19" t="n">
@@ -8105,203 +8108,203 @@
         <v>24</v>
       </c>
       <c r="H62" s="19"/>
-      <c r="I62" s="27" t="n">
+      <c r="I62" s="26" t="n">
         <f aca="false">COUNTIF(I4:I50,"&lt;&gt;Impossible")-COUNTIFS(I4:I50,"&lt;&gt;[:alpha:]*")</f>
         <v>28</v>
       </c>
-      <c r="J62" s="27"/>
+      <c r="J62" s="26"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="33"/>
-      <c r="B63" s="34" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="35" t="n">
+      <c r="C63" s="28" t="n">
         <f aca="false">100*C62/SUM($C$62:$I$62)</f>
         <v>4.41176470588235</v>
       </c>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35" t="n">
+      <c r="D63" s="28"/>
+      <c r="E63" s="28" t="n">
         <f aca="false">100*E62/SUM($C$62:$I$62)</f>
         <v>19.1176470588235</v>
       </c>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35" t="n">
+      <c r="F63" s="28"/>
+      <c r="G63" s="28" t="n">
         <f aca="false">100*G62/SUM($C$62:$I$62)</f>
         <v>35.2941176470588</v>
       </c>
-      <c r="H63" s="35"/>
-      <c r="I63" s="30" t="n">
+      <c r="H63" s="28"/>
+      <c r="I63" s="29" t="n">
         <f aca="false">100*I62/SUM($C$62:$I$62)</f>
         <v>41.1764705882353</v>
       </c>
-      <c r="J63" s="30"/>
+      <c r="J63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="33"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="37"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="36"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="29" t="n">
+      <c r="B65" s="30"/>
+      <c r="C65" s="28" t="n">
         <f aca="false">(C60+C63)</f>
         <v>4.41176470588235</v>
       </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29" t="n">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28" t="n">
         <f aca="false">(E60+E63)</f>
         <v>19.1176470588235</v>
       </c>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29" t="n">
+      <c r="F65" s="28"/>
+      <c r="G65" s="28" t="n">
         <f aca="false">(G60+G63)</f>
         <v>85.2941176470588</v>
       </c>
-      <c r="H65" s="29"/>
-      <c r="I65" s="30" t="n">
+      <c r="H65" s="28"/>
+      <c r="I65" s="29" t="n">
         <f aca="false">(I60+I63)</f>
         <v>91.1764705882353</v>
       </c>
-      <c r="J65" s="30"/>
+      <c r="J65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="29" t="n">
+      <c r="B66" s="30"/>
+      <c r="C66" s="28" t="n">
         <f aca="false">ABS(C63-C60)</f>
         <v>4.41176470588235</v>
       </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29" t="n">
+      <c r="D66" s="28"/>
+      <c r="E66" s="28" t="n">
         <f aca="false">ABS(E63-E60)</f>
         <v>19.1176470588235</v>
       </c>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29" t="n">
+      <c r="F66" s="28"/>
+      <c r="G66" s="28" t="n">
         <f aca="false">ABS(G63-G60)</f>
         <v>14.7058823529412</v>
       </c>
-      <c r="H66" s="29"/>
-      <c r="I66" s="30" t="n">
+      <c r="H66" s="28"/>
+      <c r="I66" s="29" t="n">
         <f aca="false">ABS(I63-I60)</f>
         <v>8.8235294117647</v>
       </c>
-      <c r="J66" s="30"/>
+      <c r="J66" s="29"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="29" t="n">
+      <c r="B67" s="30"/>
+      <c r="C67" s="28" t="n">
         <f aca="false">1-C66/C65</f>
         <v>0</v>
       </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29" t="n">
+      <c r="D67" s="28"/>
+      <c r="E67" s="28" t="n">
         <f aca="false">1-E66/E65</f>
         <v>0</v>
       </c>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29" t="n">
+      <c r="F67" s="28"/>
+      <c r="G67" s="28" t="n">
         <f aca="false">1-G66/G65</f>
         <v>0.827586206896552</v>
       </c>
-      <c r="H67" s="29"/>
-      <c r="I67" s="30" t="n">
+      <c r="H67" s="28"/>
+      <c r="I67" s="29" t="n">
         <f aca="false">1-I66/I65</f>
         <v>0.903225806451613</v>
       </c>
-      <c r="J67" s="30"/>
+      <c r="J67" s="29"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="18"/>
-      <c r="C68" s="29"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="38"/>
-      <c r="E68" s="29"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="38"/>
-      <c r="G68" s="29"/>
+      <c r="G68" s="37"/>
       <c r="H68" s="38"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="36"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="39" t="s">
         <v>99</v>
       </c>
       <c r="B69" s="39"/>
-      <c r="C69" s="29" t="n">
+      <c r="C69" s="28" t="n">
         <f aca="false">SUM(D4:D50)</f>
         <v>6</v>
       </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29" t="n">
+      <c r="D69" s="28"/>
+      <c r="E69" s="28" t="n">
         <f aca="false">SUM(F4:F50)</f>
         <v>29</v>
       </c>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29" t="n">
+      <c r="F69" s="28"/>
+      <c r="G69" s="28" t="n">
         <f aca="false">SUM(H4:H50)</f>
         <v>52</v>
       </c>
-      <c r="H69" s="29"/>
-      <c r="I69" s="30" t="n">
+      <c r="H69" s="28"/>
+      <c r="I69" s="29" t="n">
         <f aca="false">SUM(J4:J50)</f>
         <v>77</v>
       </c>
-      <c r="J69" s="30"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="39" t="s">
         <v>100</v>
       </c>
       <c r="B70" s="39"/>
-      <c r="C70" s="29" t="n">
+      <c r="C70" s="28" t="n">
         <f aca="false">C69*C67</f>
         <v>0</v>
       </c>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29" t="n">
+      <c r="D70" s="28"/>
+      <c r="E70" s="28" t="n">
         <f aca="false">E69*E67</f>
         <v>0</v>
       </c>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29" t="n">
+      <c r="F70" s="28"/>
+      <c r="G70" s="28" t="n">
         <f aca="false">G69*G67</f>
         <v>43.0344827586207</v>
       </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="30" t="n">
+      <c r="H70" s="28"/>
+      <c r="I70" s="29" t="n">
         <f aca="false">I69*I67</f>
         <v>69.5483870967742</v>
       </c>
-      <c r="J70" s="30"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="33"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="18"/>
-      <c r="C71" s="22"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="18"/>
-      <c r="E71" s="22"/>
+      <c r="E71" s="21"/>
       <c r="F71" s="18"/>
-      <c r="G71" s="22"/>
+      <c r="G71" s="21"/>
       <c r="H71" s="18"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="32"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="31"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="40" t="s">

</xml_diff>